<commit_message>
v5 changes; EmbassyInvoices that produce invoices from Intacct data instead of TCP
</commit_message>
<xml_diff>
--- a/data/EmployeeInfo.xlsx
+++ b/data/EmployeeInfo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dkinney/dev/midi/embassyInvoices/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2243003-0CF7-6F42-9E8F-CDD55C5E8215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FD5352-58B6-494F-B492-118041725568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="520" yWindow="500" windowWidth="23080" windowHeight="18900" xr2:uid="{8BA8A61B-9430-DC41-9FA1-1FB5F3DBB9C9}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>Financial Asst</t>
   </si>
   <si>
-    <t>Al-Assar, Anise</t>
-  </si>
-  <si>
     <t>mechanical Engineer</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>X148</t>
   </si>
   <si>
-    <t>Conner, Marc</t>
-  </si>
-  <si>
     <t>Secure Logistician</t>
   </si>
   <si>
@@ -732,6 +726,12 @@
   </si>
   <si>
     <t>SubCLIN</t>
+  </si>
+  <si>
+    <t>Conner, Marc D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al-Assar, Anise </t>
   </si>
 </sst>
 </file>
@@ -1195,8 +1195,8 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1211,31 +1211,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1255,7 +1255,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G2" s="14">
         <v>0.2</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>10</v>
+        <v>230</v>
       </c>
       <c r="B3" s="10">
         <v>11965</v>
@@ -1284,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G3" s="14">
         <v>0.2</v>
@@ -1293,12 +1293,12 @@
         <v>0</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B4" s="10">
         <v>11935</v>
@@ -1310,10 +1310,10 @@
         <v>35.22</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G4" s="14">
         <v>0.05</v>
@@ -1322,12 +1322,12 @@
         <v>0</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B5" s="10">
         <v>12002</v>
@@ -1339,10 +1339,10 @@
         <v>93.75</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G5" s="14">
         <v>0.25</v>
@@ -1351,12 +1351,12 @@
         <v>0</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B6" s="10">
         <v>11956</v>
@@ -1368,10 +1368,10 @@
         <v>35.22</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G6" s="14">
         <v>0.25</v>
@@ -1380,12 +1380,12 @@
         <v>0</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B7" s="10">
         <v>11962</v>
@@ -1400,7 +1400,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="14">
         <v>0.35</v>
@@ -1409,12 +1409,12 @@
         <v>0</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B8" s="10" t="e">
         <v>#N/A</v>
@@ -1426,7 +1426,7 @@
         <v>75</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="14">
@@ -1436,12 +1436,12 @@
         <v>0</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B9" s="10">
         <v>11938</v>
@@ -1453,10 +1453,10 @@
         <v>61.5</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G9" s="15">
         <v>0</v>
@@ -1465,12 +1465,12 @@
         <v>0</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B10" s="10">
         <v>11993</v>
@@ -1485,7 +1485,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="14">
         <v>0.35</v>
@@ -1494,12 +1494,12 @@
         <v>0</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B11" s="10">
         <v>11970</v>
@@ -1511,10 +1511,10 @@
         <v>75</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G11" s="14">
         <v>0.25</v>
@@ -1523,12 +1523,12 @@
         <v>0</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B12" s="10" t="e">
         <v>#N/A</v>
@@ -1540,7 +1540,7 @@
         <v>45.38</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="14">
@@ -1550,12 +1550,12 @@
         <v>0</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B13" s="10">
         <v>12072</v>
@@ -1567,10 +1567,10 @@
         <v>57</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G13" s="14">
         <v>0.2</v>
@@ -1579,12 +1579,12 @@
         <v>0</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B14" s="10">
         <v>11969</v>
@@ -1599,7 +1599,7 @@
         <v>7</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" s="14">
         <v>0.35</v>
@@ -1608,12 +1608,12 @@
         <v>0</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B15" s="10">
         <v>11958</v>
@@ -1628,7 +1628,7 @@
         <v>7</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="14">
         <v>0.35</v>
@@ -1637,12 +1637,12 @@
         <v>0</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>20</v>
+        <v>229</v>
       </c>
       <c r="B16" s="10">
         <v>11977</v>
@@ -1657,7 +1657,7 @@
         <v>7</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G16" s="14">
         <v>0.35</v>
@@ -1666,12 +1666,12 @@
         <v>0</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B17" s="10">
         <v>11966</v>
@@ -1683,10 +1683,10 @@
         <v>46.87</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G17" s="14">
         <v>0.25</v>
@@ -1695,12 +1695,12 @@
         <v>0</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B18" s="10">
         <v>11998</v>
@@ -1712,10 +1712,10 @@
         <v>52.5</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G18" s="14">
         <v>0.25</v>
@@ -1724,12 +1724,12 @@
         <v>0</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B19" s="10">
         <v>11996</v>
@@ -1741,10 +1741,10 @@
         <v>70.5</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G19" s="14">
         <v>0.25</v>
@@ -1753,12 +1753,12 @@
         <v>0</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B20" s="10">
         <v>11994</v>
@@ -1770,10 +1770,10 @@
         <v>63</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G20" s="14">
         <v>0</v>
@@ -1782,12 +1782,12 @@
         <v>0</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B21" s="10">
         <v>11992</v>
@@ -1799,10 +1799,10 @@
         <v>45.03</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G21" s="14">
         <v>0.25</v>
@@ -1811,12 +1811,12 @@
         <v>0</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B22" s="10">
         <v>11995</v>
@@ -1828,10 +1828,10 @@
         <v>40.5</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G22" s="14">
         <v>0</v>
@@ -1840,12 +1840,12 @@
         <v>0</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B23" s="10">
         <v>11934</v>
@@ -1860,7 +1860,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G23" s="14">
         <v>0.35</v>
@@ -1869,12 +1869,12 @@
         <v>0</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="10" t="e">
         <v>#N/A</v>
@@ -1896,12 +1896,12 @@
         <v>0</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B25" s="10">
         <v>12035</v>
@@ -1916,7 +1916,7 @@
         <v>7</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G25" s="14">
         <v>0.35</v>
@@ -1925,12 +1925,12 @@
         <v>0</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B26" s="10">
         <v>11990</v>
@@ -1945,7 +1945,7 @@
         <v>7</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G26" s="14">
         <v>0.35</v>
@@ -1954,12 +1954,12 @@
         <v>0</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="10">
         <v>11967</v>
@@ -1974,7 +1974,7 @@
         <v>7</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G27" s="14">
         <v>0.2</v>
@@ -1983,12 +1983,12 @@
         <v>0</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B28" s="10">
         <v>11939</v>
@@ -2003,7 +2003,7 @@
         <v>7</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G28" s="15">
         <v>0.35</v>
@@ -2012,12 +2012,12 @@
         <v>0</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B29" s="10">
         <v>11988</v>
@@ -2032,7 +2032,7 @@
         <v>7</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G29" s="14">
         <v>0.35</v>
@@ -2041,12 +2041,12 @@
         <v>0</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B30" s="10">
         <v>12005</v>
@@ -2058,10 +2058,10 @@
         <v>63</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G30" s="14">
         <v>0.25</v>
@@ -2070,12 +2070,12 @@
         <v>0</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B31" s="10">
         <v>11989</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32" s="10">
         <v>11968</v>
@@ -2119,7 +2119,7 @@
         <v>7</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G32" s="14">
         <v>0.35</v>
@@ -2128,12 +2128,12 @@
         <v>0</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B33" s="10" t="e">
         <v>#N/A</v>
@@ -2155,12 +2155,12 @@
         <v>0</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B34" s="10" t="e">
         <v>#N/A</v>
@@ -2172,7 +2172,7 @@
         <v>45.25</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="14">
@@ -2182,12 +2182,12 @@
         <v>0</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B35" s="10">
         <v>11973</v>
@@ -2202,7 +2202,7 @@
         <v>7</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G35" s="14">
         <v>0.35</v>
@@ -2211,12 +2211,12 @@
         <v>0</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" s="10">
         <v>11964</v>
@@ -2231,7 +2231,7 @@
         <v>7</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G36" s="14">
         <v>0.2</v>
@@ -2240,12 +2240,12 @@
         <v>0</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B37" s="10">
         <v>11963</v>
@@ -2257,10 +2257,10 @@
         <v>35.22</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G37" s="14">
         <v>0.25</v>
@@ -2269,12 +2269,12 @@
         <v>0</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B38" s="10">
         <v>11982</v>
@@ -2286,10 +2286,10 @@
         <v>55.59</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G38" s="14">
         <v>0.25</v>
@@ -2298,12 +2298,12 @@
         <v>0</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B39" s="10">
         <v>11961</v>
@@ -2315,10 +2315,10 @@
         <v>45.25</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G39" s="14">
         <v>0.2</v>
@@ -2327,12 +2327,12 @@
         <v>0</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B40" s="10">
         <v>12003</v>
@@ -2344,10 +2344,10 @@
         <v>30</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G40" s="14">
         <v>0</v>
@@ -2356,12 +2356,12 @@
         <v>0</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B41" s="10">
         <v>11946</v>
@@ -2373,10 +2373,10 @@
         <v>37.5</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G41" s="14">
         <v>0.2</v>
@@ -2385,12 +2385,12 @@
         <v>0</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B42" s="10">
         <v>11937</v>
@@ -2402,10 +2402,10 @@
         <v>58.5</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G42" s="14">
         <v>0.2</v>
@@ -2414,12 +2414,12 @@
         <v>0</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B43" s="10">
         <v>11950</v>
@@ -2434,7 +2434,7 @@
         <v>7</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G43" s="15">
         <v>0.35</v>
@@ -2443,12 +2443,12 @@
         <v>0</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B44" s="10">
         <v>11951</v>
@@ -2463,7 +2463,7 @@
         <v>7</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G44" s="15">
         <v>0.35</v>
@@ -2472,12 +2472,12 @@
         <v>0</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B45" s="10">
         <v>11957</v>
@@ -2492,7 +2492,7 @@
         <v>7</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G45" s="14">
         <v>0.35</v>
@@ -2501,12 +2501,12 @@
         <v>0</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B46" s="10">
         <v>11987</v>
@@ -2518,10 +2518,10 @@
         <v>49.32</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G46" s="14">
         <v>0.25</v>
@@ -2530,12 +2530,12 @@
         <v>0</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B47" s="10">
         <v>11974</v>
@@ -2547,10 +2547,10 @@
         <v>35.22</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G47" s="14">
         <v>0.2</v>
@@ -2559,12 +2559,12 @@
         <v>0</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B48" s="10">
         <v>11997</v>
@@ -2579,7 +2579,7 @@
         <v>7</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G48" s="14">
         <v>0.35</v>
@@ -2588,12 +2588,12 @@
         <v>0</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B49" s="10">
         <v>12077</v>
@@ -2608,7 +2608,7 @@
         <v>7</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G49" s="14">
         <v>0.35</v>
@@ -2617,12 +2617,12 @@
         <v>0</v>
       </c>
       <c r="I49" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B50" s="10" t="e">
         <v>#N/A</v>
@@ -2644,12 +2644,12 @@
         <v>0</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B51" s="10">
         <v>11955</v>
@@ -2661,10 +2661,10 @@
         <v>49.32</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G51" s="15">
         <v>0.1</v>
@@ -2673,12 +2673,12 @@
         <v>0</v>
       </c>
       <c r="I51" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B52" s="10">
         <v>11984</v>
@@ -2690,10 +2690,10 @@
         <v>55.5</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G52" s="14">
         <v>0</v>
@@ -2702,12 +2702,12 @@
         <v>0</v>
       </c>
       <c r="I52" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B53" s="10" t="e">
         <v>#N/A</v>
@@ -2719,7 +2719,7 @@
         <v>58.35</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F53" s="10"/>
       <c r="G53" s="14">
@@ -2729,12 +2729,12 @@
         <v>0</v>
       </c>
       <c r="I53" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B54" s="10" t="e">
         <v>#N/A</v>
@@ -2746,7 +2746,7 @@
         <v>36</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F54" s="10"/>
       <c r="G54" s="14">
@@ -2756,12 +2756,12 @@
         <v>0</v>
       </c>
       <c r="I54" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B55" s="10">
         <v>11976</v>
@@ -2773,10 +2773,10 @@
         <v>39</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G55" s="14">
         <v>0.25</v>
@@ -2785,12 +2785,12 @@
         <v>0</v>
       </c>
       <c r="I55" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B56" s="10">
         <v>11952</v>
@@ -2805,7 +2805,7 @@
         <v>7</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G56" s="15">
         <v>0.35</v>
@@ -2814,12 +2814,12 @@
         <v>0</v>
       </c>
       <c r="I56" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B57" s="10">
         <v>11936</v>
@@ -2831,10 +2831,10 @@
         <v>48</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G57" s="14">
         <v>0.25</v>
@@ -2843,12 +2843,12 @@
         <v>0</v>
       </c>
       <c r="I57" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B58" s="10">
         <v>11959</v>
@@ -2863,7 +2863,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G58" s="14">
         <v>0.35</v>
@@ -2872,12 +2872,12 @@
         <v>0</v>
       </c>
       <c r="I58" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B59" s="10">
         <v>11975</v>
@@ -2892,7 +2892,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G59" s="14">
         <v>0.35</v>
@@ -2901,12 +2901,12 @@
         <v>0</v>
       </c>
       <c r="I59" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B60" s="10">
         <v>11949</v>
@@ -2918,10 +2918,10 @@
         <v>75</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G60" s="14">
         <v>0.2</v>
@@ -2930,12 +2930,12 @@
         <v>0</v>
       </c>
       <c r="I60" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B61" s="10" t="e">
         <v>#N/A</v>
@@ -2947,7 +2947,7 @@
         <v>49.79</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="14">
@@ -2957,12 +2957,12 @@
         <v>0</v>
       </c>
       <c r="I61" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B62" s="10">
         <v>12010</v>
@@ -2977,7 +2977,7 @@
         <v>7</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G62" s="14">
         <v>0.35</v>
@@ -2986,12 +2986,12 @@
         <v>0</v>
       </c>
       <c r="I62" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B63" s="10">
         <v>11942</v>
@@ -3006,7 +3006,7 @@
         <v>7</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G63" s="15">
         <v>0.35</v>
@@ -3015,12 +3015,12 @@
         <v>0</v>
       </c>
       <c r="I63" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B64" s="10">
         <v>12006</v>
@@ -3035,7 +3035,7 @@
         <v>7</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G64" s="14">
         <v>0.35</v>
@@ -3044,12 +3044,12 @@
         <v>0</v>
       </c>
       <c r="I64" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B65" s="10">
         <v>11971</v>
@@ -3061,10 +3061,10 @@
         <v>49.5</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G65" s="14">
         <v>0.2</v>
@@ -3078,7 +3078,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B66" s="10">
         <v>11991</v>
@@ -3093,7 +3093,7 @@
         <v>7</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G66" s="14">
         <v>0.35</v>
@@ -3102,12 +3102,12 @@
         <v>0</v>
       </c>
       <c r="I66" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B67" s="10" t="e">
         <v>#N/A</v>
@@ -3129,12 +3129,12 @@
         <v>0</v>
       </c>
       <c r="I67" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B68" s="10">
         <v>11944</v>
@@ -3146,10 +3146,10 @@
         <v>30</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G68" s="15">
         <v>0</v>
@@ -3158,12 +3158,12 @@
         <v>0</v>
       </c>
       <c r="I68" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B69" s="10">
         <v>11953</v>
@@ -3175,7 +3175,7 @@
         <v>44.93</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F69" s="10" t="s">
         <v>6</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B70" s="10">
         <v>11978</v>
@@ -3204,10 +3204,10 @@
         <v>90</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G70" s="14">
         <v>0.25</v>
@@ -3216,12 +3216,12 @@
         <v>0</v>
       </c>
       <c r="I70" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B71" s="10">
         <v>11986</v>
@@ -3233,10 +3233,10 @@
         <v>48.38</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G71" s="14">
         <v>0.05</v>
@@ -3245,12 +3245,12 @@
         <v>0</v>
       </c>
       <c r="I71" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B72" s="10">
         <v>11985</v>
@@ -3262,10 +3262,10 @@
         <v>75</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G72" s="14">
         <v>0.05</v>
@@ -3274,12 +3274,12 @@
         <v>0</v>
       </c>
       <c r="I72" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B73" s="10">
         <v>11981</v>
@@ -3294,7 +3294,7 @@
         <v>7</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G73" s="14">
         <v>0.35</v>
@@ -3303,12 +3303,12 @@
         <v>0</v>
       </c>
       <c r="I73" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B74" s="10">
         <v>12007</v>
@@ -3320,10 +3320,10 @@
         <v>75</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G74" s="14">
         <v>0.2</v>
@@ -3332,12 +3332,12 @@
         <v>0</v>
       </c>
       <c r="I74" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B75" s="10">
         <v>11804</v>
@@ -3352,7 +3352,7 @@
         <v>7</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G75" s="14">
         <v>0</v>
@@ -3361,12 +3361,12 @@
         <v>0</v>
       </c>
       <c r="I75" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B76" s="10">
         <v>11943</v>
@@ -3378,10 +3378,10 @@
         <v>30</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G76" s="14">
         <v>0.05</v>
@@ -3390,12 +3390,12 @@
         <v>0</v>
       </c>
       <c r="I76" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B77" s="10">
         <v>11947</v>
@@ -3410,7 +3410,7 @@
         <v>7</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G77" s="15">
         <v>0.35</v>
@@ -3419,12 +3419,12 @@
         <v>0</v>
       </c>
       <c r="I77" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B78" s="10" t="e">
         <v>#N/A</v>
@@ -3446,12 +3446,12 @@
         <v>0</v>
       </c>
       <c r="I78" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B79" s="10" t="e">
         <v>#N/A</v>
@@ -3473,12 +3473,12 @@
         <v>0</v>
       </c>
       <c r="I79" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B80" s="10">
         <v>11948</v>
@@ -3507,7 +3507,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B81" s="10">
         <v>11940</v>
@@ -3519,10 +3519,10 @@
         <v>75</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G81" s="14">
         <v>0.25</v>
@@ -3531,12 +3531,12 @@
         <v>0</v>
       </c>
       <c r="I81" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B82" s="10">
         <v>12042</v>
@@ -3548,10 +3548,10 @@
         <v>49.32</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G82" s="14">
         <v>0.25</v>
@@ -3560,12 +3560,12 @@
         <v>0</v>
       </c>
       <c r="I82" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B83" s="10">
         <v>11972</v>
@@ -3587,12 +3587,12 @@
         <v>0</v>
       </c>
       <c r="I83" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B84" s="10">
         <v>11945</v>
@@ -3604,10 +3604,10 @@
         <v>75</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G84" s="14">
         <v>0.25</v>
@@ -3616,12 +3616,12 @@
         <v>0</v>
       </c>
       <c r="I84" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B85" s="10">
         <v>11941</v>
@@ -3633,10 +3633,10 @@
         <v>76.5</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F85" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G85" s="14">
         <v>0.2</v>
@@ -3645,12 +3645,12 @@
         <v>0</v>
       </c>
       <c r="I85" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B86" s="10">
         <v>12000</v>
@@ -3665,7 +3665,7 @@
         <v>7</v>
       </c>
       <c r="F86" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G86" s="14">
         <v>0.35</v>
@@ -3679,7 +3679,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B87" s="10">
         <v>12001</v>
@@ -3694,7 +3694,7 @@
         <v>7</v>
       </c>
       <c r="F87" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G87" s="14">
         <v>0.35</v>
@@ -3703,12 +3703,12 @@
         <v>0</v>
       </c>
       <c r="I87" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B88" s="10">
         <v>11954</v>
@@ -3723,7 +3723,7 @@
         <v>7</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G88" s="15">
         <v>0.35</v>
@@ -3732,12 +3732,12 @@
         <v>0</v>
       </c>
       <c r="I88" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B89" s="10">
         <v>11980</v>
@@ -3752,7 +3752,7 @@
         <v>7</v>
       </c>
       <c r="F89" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G89" s="14">
         <v>0.2</v>
@@ -3761,12 +3761,12 @@
         <v>0</v>
       </c>
       <c r="I89" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B90" s="10" t="e">
         <v>#N/A</v>
@@ -3803,12 +3803,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3950,15 +3947,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D225599-449A-4087-B2E0-99B33D8F971E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF938FBE-B74B-40A9-9020-D4131E4167C9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="771c2b47-ec96-4714-98ff-1fee956584f3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3982,17 +3990,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF938FBE-B74B-40A9-9020-D4131E4167C9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D225599-449A-4087-B2E0-99B33D8F971E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="771c2b47-ec96-4714-98ff-1fee956584f3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
check for employees who do not join with rates because of their name
</commit_message>
<xml_diff>
--- a/data/EmployeeInfo.xlsx
+++ b/data/EmployeeInfo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dkinney/dev/midi/embassyInvoices/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FD5352-58B6-494F-B492-118041725568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881443D7-8A98-6A42-8041-B09DF5BAF0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="520" yWindow="500" windowWidth="23080" windowHeight="18900" xr2:uid="{8BA8A61B-9430-DC41-9FA1-1FB5F3DBB9C9}"/>
   </bookViews>
@@ -131,9 +131,6 @@
     <t>RSO Security Liaison</t>
   </si>
   <si>
-    <t>Harvey, Kerlin</t>
-  </si>
-  <si>
     <t>auto mechanic</t>
   </si>
   <si>
@@ -732,6 +729,9 @@
   </si>
   <si>
     <t xml:space="preserve">Al-Assar, Anise </t>
+  </si>
+  <si>
+    <t>Harvey, Kerlin J</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1196,7 @@
   <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1211,31 +1211,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="I1" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1255,7 +1255,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G2" s="14">
         <v>0.2</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B3" s="10">
         <v>11965</v>
@@ -1284,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G3" s="14">
         <v>0.2</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B4" s="10">
         <v>11935</v>
@@ -1310,10 +1310,10 @@
         <v>35.22</v>
       </c>
       <c r="E4" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>81</v>
       </c>
       <c r="G4" s="14">
         <v>0.05</v>
@@ -1322,12 +1322,12 @@
         <v>0</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B5" s="10">
         <v>12002</v>
@@ -1339,10 +1339,10 @@
         <v>93.75</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5" s="14">
         <v>0.25</v>
@@ -1351,12 +1351,12 @@
         <v>0</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B6" s="10">
         <v>11956</v>
@@ -1368,10 +1368,10 @@
         <v>35.22</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G6" s="14">
         <v>0.25</v>
@@ -1380,12 +1380,12 @@
         <v>0</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B7" s="10">
         <v>11962</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" s="10" t="e">
         <v>#N/A</v>
@@ -1426,7 +1426,7 @@
         <v>75</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="14">
@@ -1441,7 +1441,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B9" s="10">
         <v>11938</v>
@@ -1453,10 +1453,10 @@
         <v>61.5</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G9" s="15">
         <v>0</v>
@@ -1465,12 +1465,12 @@
         <v>0</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B10" s="10">
         <v>11993</v>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B11" s="10">
         <v>11970</v>
@@ -1511,10 +1511,10 @@
         <v>75</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G11" s="14">
         <v>0.25</v>
@@ -1523,12 +1523,12 @@
         <v>0</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" s="10" t="e">
         <v>#N/A</v>
@@ -1540,7 +1540,7 @@
         <v>45.38</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="14">
@@ -1550,12 +1550,12 @@
         <v>0</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B13" s="10">
         <v>12072</v>
@@ -1567,10 +1567,10 @@
         <v>57</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G13" s="14">
         <v>0.2</v>
@@ -1579,12 +1579,12 @@
         <v>0</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B14" s="10">
         <v>11969</v>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B15" s="10">
         <v>11958</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B16" s="10">
         <v>11977</v>
@@ -1657,7 +1657,7 @@
         <v>7</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G16" s="14">
         <v>0.35</v>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B17" s="10">
         <v>11966</v>
@@ -1683,10 +1683,10 @@
         <v>46.87</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G17" s="14">
         <v>0.25</v>
@@ -1695,12 +1695,12 @@
         <v>0</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B18" s="10">
         <v>11998</v>
@@ -1712,10 +1712,10 @@
         <v>52.5</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G18" s="14">
         <v>0.25</v>
@@ -1724,12 +1724,12 @@
         <v>0</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B19" s="10">
         <v>11996</v>
@@ -1741,10 +1741,10 @@
         <v>70.5</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G19" s="14">
         <v>0.25</v>
@@ -1753,12 +1753,12 @@
         <v>0</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B20" s="10">
         <v>11994</v>
@@ -1770,10 +1770,10 @@
         <v>63</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" s="14">
         <v>0</v>
@@ -1782,12 +1782,12 @@
         <v>0</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B21" s="10">
         <v>11992</v>
@@ -1799,10 +1799,10 @@
         <v>45.03</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G21" s="14">
         <v>0.25</v>
@@ -1811,12 +1811,12 @@
         <v>0</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B22" s="10">
         <v>11995</v>
@@ -1828,10 +1828,10 @@
         <v>40.5</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G22" s="14">
         <v>0</v>
@@ -1840,12 +1840,12 @@
         <v>0</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B23" s="10">
         <v>11934</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B25" s="10">
         <v>12035</v>
@@ -1916,7 +1916,7 @@
         <v>7</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G25" s="14">
         <v>0.35</v>
@@ -1930,7 +1930,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B26" s="10">
         <v>11990</v>
@@ -1974,7 +1974,7 @@
         <v>7</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G27" s="14">
         <v>0.2</v>
@@ -1988,7 +1988,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B28" s="10">
         <v>11939</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B29" s="10">
         <v>11988</v>
@@ -2032,7 +2032,7 @@
         <v>7</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G29" s="14">
         <v>0.35</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B30" s="10">
         <v>12005</v>
@@ -2058,10 +2058,10 @@
         <v>63</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G30" s="14">
         <v>0.25</v>
@@ -2070,12 +2070,12 @@
         <v>0</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B31" s="10">
         <v>11989</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>30</v>
+        <v>230</v>
       </c>
       <c r="B32" s="10">
         <v>11968</v>
@@ -2119,7 +2119,7 @@
         <v>7</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G32" s="14">
         <v>0.35</v>
@@ -2128,12 +2128,12 @@
         <v>0</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="10" t="e">
         <v>#N/A</v>
@@ -2160,7 +2160,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" s="10" t="e">
         <v>#N/A</v>
@@ -2172,7 +2172,7 @@
         <v>45.25</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="14">
@@ -2182,12 +2182,12 @@
         <v>0</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B35" s="10">
         <v>11973</v>
@@ -2202,7 +2202,7 @@
         <v>7</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G35" s="14">
         <v>0.35</v>
@@ -2211,12 +2211,12 @@
         <v>0</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="10">
         <v>11964</v>
@@ -2231,7 +2231,7 @@
         <v>7</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G36" s="14">
         <v>0.2</v>
@@ -2240,12 +2240,12 @@
         <v>0</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B37" s="10">
         <v>11963</v>
@@ -2257,10 +2257,10 @@
         <v>35.22</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G37" s="14">
         <v>0.25</v>
@@ -2269,12 +2269,12 @@
         <v>0</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B38" s="10">
         <v>11982</v>
@@ -2286,10 +2286,10 @@
         <v>55.59</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G38" s="14">
         <v>0.25</v>
@@ -2298,12 +2298,12 @@
         <v>0</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B39" s="10">
         <v>11961</v>
@@ -2315,10 +2315,10 @@
         <v>45.25</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G39" s="14">
         <v>0.2</v>
@@ -2332,7 +2332,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B40" s="10">
         <v>12003</v>
@@ -2344,10 +2344,10 @@
         <v>30</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G40" s="14">
         <v>0</v>
@@ -2356,12 +2356,12 @@
         <v>0</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B41" s="10">
         <v>11946</v>
@@ -2373,10 +2373,10 @@
         <v>37.5</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G41" s="14">
         <v>0.2</v>
@@ -2385,12 +2385,12 @@
         <v>0</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B42" s="10">
         <v>11937</v>
@@ -2402,10 +2402,10 @@
         <v>58.5</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G42" s="14">
         <v>0.2</v>
@@ -2414,12 +2414,12 @@
         <v>0</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B43" s="10">
         <v>11950</v>
@@ -2434,7 +2434,7 @@
         <v>7</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G43" s="15">
         <v>0.35</v>
@@ -2443,12 +2443,12 @@
         <v>0</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B44" s="10">
         <v>11951</v>
@@ -2463,7 +2463,7 @@
         <v>7</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G44" s="15">
         <v>0.35</v>
@@ -2472,12 +2472,12 @@
         <v>0</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" s="10">
         <v>11957</v>
@@ -2492,7 +2492,7 @@
         <v>7</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G45" s="14">
         <v>0.35</v>
@@ -2501,12 +2501,12 @@
         <v>0</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B46" s="10">
         <v>11987</v>
@@ -2518,10 +2518,10 @@
         <v>49.32</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G46" s="14">
         <v>0.25</v>
@@ -2530,12 +2530,12 @@
         <v>0</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B47" s="10">
         <v>11974</v>
@@ -2547,10 +2547,10 @@
         <v>35.22</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G47" s="14">
         <v>0.2</v>
@@ -2559,12 +2559,12 @@
         <v>0</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B48" s="10">
         <v>11997</v>
@@ -2593,7 +2593,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B49" s="10">
         <v>12077</v>
@@ -2608,7 +2608,7 @@
         <v>7</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G49" s="14">
         <v>0.35</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B50" s="10" t="e">
         <v>#N/A</v>
@@ -2644,12 +2644,12 @@
         <v>0</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B51" s="10">
         <v>11955</v>
@@ -2661,10 +2661,10 @@
         <v>49.32</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G51" s="15">
         <v>0.1</v>
@@ -2673,12 +2673,12 @@
         <v>0</v>
       </c>
       <c r="I51" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B52" s="10">
         <v>11984</v>
@@ -2690,10 +2690,10 @@
         <v>55.5</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G52" s="14">
         <v>0</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B53" s="10" t="e">
         <v>#N/A</v>
@@ -2719,7 +2719,7 @@
         <v>58.35</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F53" s="10"/>
       <c r="G53" s="14">
@@ -2734,7 +2734,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="10" t="e">
         <v>#N/A</v>
@@ -2746,7 +2746,7 @@
         <v>36</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F54" s="10"/>
       <c r="G54" s="14">
@@ -2756,12 +2756,12 @@
         <v>0</v>
       </c>
       <c r="I54" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B55" s="10">
         <v>11976</v>
@@ -2773,10 +2773,10 @@
         <v>39</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G55" s="14">
         <v>0.25</v>
@@ -2785,12 +2785,12 @@
         <v>0</v>
       </c>
       <c r="I55" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B56" s="10">
         <v>11952</v>
@@ -2805,7 +2805,7 @@
         <v>7</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G56" s="15">
         <v>0.35</v>
@@ -2814,12 +2814,12 @@
         <v>0</v>
       </c>
       <c r="I56" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B57" s="10">
         <v>11936</v>
@@ -2831,10 +2831,10 @@
         <v>48</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G57" s="14">
         <v>0.25</v>
@@ -2843,12 +2843,12 @@
         <v>0</v>
       </c>
       <c r="I57" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B58" s="10">
         <v>11959</v>
@@ -2863,7 +2863,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G58" s="14">
         <v>0.35</v>
@@ -2872,12 +2872,12 @@
         <v>0</v>
       </c>
       <c r="I58" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B59" s="10">
         <v>11975</v>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B60" s="10">
         <v>11949</v>
@@ -2918,10 +2918,10 @@
         <v>75</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G60" s="14">
         <v>0.2</v>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B61" s="10" t="e">
         <v>#N/A</v>
@@ -2947,7 +2947,7 @@
         <v>49.79</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="14">
@@ -2957,12 +2957,12 @@
         <v>0</v>
       </c>
       <c r="I61" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B62" s="10">
         <v>12010</v>
@@ -2977,7 +2977,7 @@
         <v>7</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G62" s="14">
         <v>0.35</v>
@@ -2991,7 +2991,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B63" s="10">
         <v>11942</v>
@@ -3006,7 +3006,7 @@
         <v>7</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G63" s="15">
         <v>0.35</v>
@@ -3015,12 +3015,12 @@
         <v>0</v>
       </c>
       <c r="I63" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B64" s="10">
         <v>12006</v>
@@ -3035,7 +3035,7 @@
         <v>7</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G64" s="14">
         <v>0.35</v>
@@ -3044,12 +3044,12 @@
         <v>0</v>
       </c>
       <c r="I64" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B65" s="10">
         <v>11971</v>
@@ -3061,10 +3061,10 @@
         <v>49.5</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G65" s="14">
         <v>0.2</v>
@@ -3078,7 +3078,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B66" s="10">
         <v>11991</v>
@@ -3093,7 +3093,7 @@
         <v>7</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G66" s="14">
         <v>0.35</v>
@@ -3102,12 +3102,12 @@
         <v>0</v>
       </c>
       <c r="I66" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B67" s="10" t="e">
         <v>#N/A</v>
@@ -3134,7 +3134,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B68" s="10">
         <v>11944</v>
@@ -3146,10 +3146,10 @@
         <v>30</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G68" s="15">
         <v>0</v>
@@ -3158,12 +3158,12 @@
         <v>0</v>
       </c>
       <c r="I68" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B69" s="10">
         <v>11953</v>
@@ -3175,7 +3175,7 @@
         <v>44.93</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F69" s="10" t="s">
         <v>6</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B70" s="10">
         <v>11978</v>
@@ -3204,10 +3204,10 @@
         <v>90</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G70" s="14">
         <v>0.25</v>
@@ -3216,12 +3216,12 @@
         <v>0</v>
       </c>
       <c r="I70" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B71" s="10">
         <v>11986</v>
@@ -3233,10 +3233,10 @@
         <v>48.38</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G71" s="14">
         <v>0.05</v>
@@ -3245,12 +3245,12 @@
         <v>0</v>
       </c>
       <c r="I71" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B72" s="10">
         <v>11985</v>
@@ -3262,10 +3262,10 @@
         <v>75</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G72" s="14">
         <v>0.05</v>
@@ -3274,12 +3274,12 @@
         <v>0</v>
       </c>
       <c r="I72" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B73" s="10">
         <v>11981</v>
@@ -3294,7 +3294,7 @@
         <v>7</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G73" s="14">
         <v>0.35</v>
@@ -3303,12 +3303,12 @@
         <v>0</v>
       </c>
       <c r="I73" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B74" s="10">
         <v>12007</v>
@@ -3320,10 +3320,10 @@
         <v>75</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G74" s="14">
         <v>0.2</v>
@@ -3332,12 +3332,12 @@
         <v>0</v>
       </c>
       <c r="I74" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B75" s="10">
         <v>11804</v>
@@ -3352,21 +3352,21 @@
         <v>7</v>
       </c>
       <c r="F75" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G75" s="14">
+        <v>0</v>
+      </c>
+      <c r="H75" s="14">
+        <v>0</v>
+      </c>
+      <c r="I75" s="13" t="s">
         <v>133</v>
-      </c>
-      <c r="G75" s="14">
-        <v>0</v>
-      </c>
-      <c r="H75" s="14">
-        <v>0</v>
-      </c>
-      <c r="I75" s="13" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B76" s="10">
         <v>11943</v>
@@ -3378,10 +3378,10 @@
         <v>30</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G76" s="14">
         <v>0.05</v>
@@ -3390,12 +3390,12 @@
         <v>0</v>
       </c>
       <c r="I76" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B77" s="10">
         <v>11947</v>
@@ -3410,7 +3410,7 @@
         <v>7</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G77" s="15">
         <v>0.35</v>
@@ -3424,7 +3424,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B78" s="10" t="e">
         <v>#N/A</v>
@@ -3451,7 +3451,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B79" s="10" t="e">
         <v>#N/A</v>
@@ -3473,12 +3473,12 @@
         <v>0</v>
       </c>
       <c r="I79" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B80" s="10">
         <v>11948</v>
@@ -3507,7 +3507,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B81" s="10">
         <v>11940</v>
@@ -3519,10 +3519,10 @@
         <v>75</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G81" s="14">
         <v>0.25</v>
@@ -3531,12 +3531,12 @@
         <v>0</v>
       </c>
       <c r="I81" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B82" s="10">
         <v>12042</v>
@@ -3548,10 +3548,10 @@
         <v>49.32</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G82" s="14">
         <v>0.25</v>
@@ -3560,12 +3560,12 @@
         <v>0</v>
       </c>
       <c r="I82" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B83" s="10">
         <v>11972</v>
@@ -3587,12 +3587,12 @@
         <v>0</v>
       </c>
       <c r="I83" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B84" s="10">
         <v>11945</v>
@@ -3604,10 +3604,10 @@
         <v>75</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G84" s="14">
         <v>0.25</v>
@@ -3621,7 +3621,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B85" s="10">
         <v>11941</v>
@@ -3633,10 +3633,10 @@
         <v>76.5</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F85" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G85" s="14">
         <v>0.2</v>
@@ -3645,12 +3645,12 @@
         <v>0</v>
       </c>
       <c r="I85" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B86" s="10">
         <v>12000</v>
@@ -3665,7 +3665,7 @@
         <v>7</v>
       </c>
       <c r="F86" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G86" s="14">
         <v>0.35</v>
@@ -3679,7 +3679,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B87" s="10">
         <v>12001</v>
@@ -3694,7 +3694,7 @@
         <v>7</v>
       </c>
       <c r="F87" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G87" s="14">
         <v>0.35</v>
@@ -3703,12 +3703,12 @@
         <v>0</v>
       </c>
       <c r="I87" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B88" s="10">
         <v>11954</v>
@@ -3723,7 +3723,7 @@
         <v>7</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G88" s="15">
         <v>0.35</v>
@@ -3732,12 +3732,12 @@
         <v>0</v>
       </c>
       <c r="I88" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B89" s="10">
         <v>11980</v>
@@ -3752,7 +3752,7 @@
         <v>7</v>
       </c>
       <c r="F89" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G89" s="14">
         <v>0.2</v>
@@ -3761,12 +3761,12 @@
         <v>0</v>
       </c>
       <c r="I89" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B90" s="10" t="e">
         <v>#N/A</v>
@@ -3803,12 +3803,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC60A8BE1883024EA8FB57797847A85B" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dd73aacbb958d3880fe43d499e9ad3d7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="771c2b47-ec96-4714-98ff-1fee956584f3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f4333f356e4faef7282ab556c8438869" ns2:_="">
     <xsd:import namespace="771c2b47-ec96-4714-98ff-1fee956584f3"/>
@@ -3946,6 +3940,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3956,22 +3956,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF938FBE-B74B-40A9-9020-D4131E4167C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="771c2b47-ec96-4714-98ff-1fee956584f3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C432C7B-AA2C-4E28-8EA2-AA7FEB71A317}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3989,6 +3973,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF938FBE-B74B-40A9-9020-D4131E4167C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="771c2b47-ec96-4714-98ff-1fee956584f3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D225599-449A-4087-B2E0-99B33D8F971E}">
   <ds:schemaRefs>

</xml_diff>